<commit_message>
fixes related to locator visibility
</commit_message>
<xml_diff>
--- a/xlsx-reports/job_applications.xlsx
+++ b/xlsx-reports/job_applications.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Title</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Java Full Stack Developer- Charlotte, NC</t>
+    <t>Java Full-Stack Developer</t>
   </si>
   <si>
     <t>❌</t>
@@ -37,37 +37,31 @@
     <t>✅</t>
   </si>
   <si>
-    <t>https://www.dice.com/job-detail/142cfc98-dfb1-4039-adba-9a898d58c68d</t>
-  </si>
-  <si>
-    <t>Java Full Stack Developer</t>
-  </si>
-  <si>
-    <t>https://www.dice.com/job-detail/19b5f1c4-27bf-4b6e-8095-1bad11ce5857</t>
-  </si>
-  <si>
-    <t>Java Developer / Java Full stack Developer/ Software Developer</t>
-  </si>
-  <si>
-    <t>https://www.dice.com/job-detail/709ac53d-8091-4cff-86bc-8e8cb2ed87de</t>
-  </si>
-  <si>
-    <t>https://www.dice.com/job-detail/f65dc071-2b55-43e5-9e75-efe825f5193c</t>
-  </si>
-  <si>
-    <t>Java Full Stack Developer (10+ years)</t>
-  </si>
-  <si>
-    <t>https://www.dice.com/application-submitted?eyJjb3JyZWxhdGlvbl9pZCI6ImFhNDczM2YyLTgyMGItNDA1NC04YzIyLWIxZDk0ODE3YWRjOCIsImRqdlZlcnNpb24iOiJuZXciLCJqb2JJZCI6ImMyMDQ0MGJiLTUzMTMtNDljMS04MjIwLWY1ZGJiMmQ0NTZmYyIsImpvYlVybCI6Imh0dHBzOi8vd3d3LmRpY2UuY29tL2pvYi1kZXRhaWwvYzIwNDQwYmItNTMxMy00OWMxLTgyMjAtZjVkYmIyZDQ1NmZjIiwiam9iVGl0bGUiOiJKYXZhIEZ1bGwgU3RhY2sgRGV2ZWxvcGVyICgxMCsgeWVhcnMpIiwic2VhcmNoTGluayI6IiJ9</t>
+    <t>https://www.dice.com/application-submitted?eyJjb3JyZWxhdGlvbl9pZCI6ImI3ZGMwMDBjLTFmNzItNGM5MS1iNDZhLTQ4MDlmYTFmODM3ZiIsImRqdlZlcnNpb24iOiJuZXciLCJqb2JJZCI6ImRmMjM1NzBiLTVkM2EtNGZjYy05YWU2LTE3NWJlNDVlOTRkOSIsImpvYlVybCI6Imh0dHBzOi8vd3d3LmRpY2UuY29tL2pvYi1kZXRhaWwvZGYyMzU3MGItNWQzYS00ZmNjLTlhZTYtMTc1YmU0NWU5NGQ5Iiwiam9iVGl0bGUiOiJKYXZhIEZ1bGwtU3RhY2sgRGV2ZWxvcGVyIiwic2VhcmNoTGluayI6IiJ9</t>
+  </si>
+  <si>
+    <t>Fullstack Java Developer- Hybrid</t>
+  </si>
+  <si>
+    <t>https://www.dice.com/application-submitted?eyJjb3JyZWxhdGlvbl9pZCI6ImJlNWEyNWE0LTgyY2QtNDljYi04MGQ5LWZhNzFlNzlhYmI2YyIsImRqdlZlcnNpb24iOiJuZXciLCJqb2JJZCI6Ijk2YzdmYzZkLTAwOWMtNDI4Yi1iMGRkLTE0NWJkMjE3ZTExNyIsImpvYlVybCI6Imh0dHBzOi8vd3d3LmRpY2UuY29tL2pvYi1kZXRhaWwvOTZjN2ZjNmQtMDA5Yy00MjhiLWIwZGQtMTQ1YmQyMTdlMTE3Iiwiam9iVGl0bGUiOiJGdWxsc3RhY2sgSmF2YSBEZXZlbG9wZXItIEh5YnJpZCIsInNlYXJjaExpbmsiOiIifQ==</t>
+  </si>
+  <si>
+    <t>JAVA Reactjs Fullstack Developer - Local candidates preferred</t>
+  </si>
+  <si>
+    <t>https://www.dice.com/application-submitted?eyJjb3JyZWxhdGlvbl9pZCI6IjdjMzNhYTlmLTk4NjgtNDRiYS05NDEzLTI4ZDgwOWE0M2IyOCIsImRqdlZlcnNpb24iOiJuZXciLCJqb2JJZCI6ImYzN2EzMjVmLWQxNTktNDk2My04NDJlLTZkYmFjMGFlYzUxZCIsImpvYlVybCI6Imh0dHBzOi8vd3d3LmRpY2UuY29tL2pvYi1kZXRhaWwvZjM3YTMyNWYtZDE1OS00OTYzLTg0MmUtNmRiYWMwYWVjNTFkIiwiam9iVGl0bGUiOiJKQVZBIFJlYWN0anMgRnVsbHN0YWNrIERldmVsb3BlciAtIExvY2FsIGNhbmRpZGF0ZXMgcHJlZmVycmVkIiwic2VhcmNoTGluayI6IiJ9</t>
+  </si>
+  <si>
+    <t>Java Full stack dev with AWS , React , Python , Terraform , Jetstream UX - Dallas TX (1) , Hyderabad - Offshore (1) - Both Onsite positions</t>
+  </si>
+  <si>
+    <t>https://www.dice.com/application-submitted?eyJjb3JyZWxhdGlvbl9pZCI6IjEyNjdmODY3LTNkOTgtNGFiOC1hYzRmLWIwOWFhNDUyMWRiNCIsImRqdlZlcnNpb24iOiJuZXciLCJqb2JJZCI6IjZmNTQzZDY3LTVlMDctNGEyMC1hMDBiLWVmOWRhOGUyYzg3MCIsImpvYlVybCI6Imh0dHBzOi8vd3d3LmRpY2UuY29tL2pvYi1kZXRhaWwvNmY1NDNkNjctNWUwNy00YTIwLWEwMGItZWY5ZGE4ZTJjODcwIiwiam9iVGl0bGUiOiJKYXZhIEZ1bGwgc3RhY2sgZGV2IHdpdGggQVdTICwgUmVhY3QgLCBQeXRob24gLCBUZXJyYWZvcm0gLCBKZXRzdHJlYW0gVVggLSBEYWxsYXMgVFggKDEpICwgSHlkZXJhYmFkIC0gT2Zmc2hvcmUgKDEpIC0gQm90aCBPbnNpdGUgcG9zaXRpb25zIiwic2VhcmNoTGluayI6IiJ9</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>4</t>
@@ -450,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
@@ -484,10 +478,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -501,10 +495,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -518,10 +512,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -529,53 +523,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>